<commit_message>
planning updated also changed the database to fontys
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\ASP.NETCinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246D544A-BF6D-4E7F-A1F3-2934A0EDA3A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D759FD6-C199-4C34-85F0-9B35C8BDD5D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22E80722-1DB3-4D4A-B95F-931B24953C16}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Sprint</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Dit heb ik vaker gedaan dus dit zal niet heel lang moeten duren.</t>
+  </si>
+  <si>
+    <t>Totaal</t>
+  </si>
+  <si>
+    <t>Bezig (Niet af)</t>
   </si>
 </sst>
 </file>
@@ -171,8 +177,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -315,7 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -356,20 +362,23 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -689,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B06F840-217A-487E-A4A4-1D61301F5C6F}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -889,18 +898,24 @@
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="5">
+        <v>43500</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43637</v>
+      </c>
       <c r="F8" s="14">
         <f>SUM(F2:F7)</f>
         <v>19.142857142857142</v>
       </c>
       <c r="G8" s="2">
-        <f>SUM(G2:G6)</f>
-        <v>175</v>
+        <f>SUM(G2:G7)</f>
+        <v>210</v>
       </c>
       <c r="H8" s="14">
         <f>SUM(H2:H6)</f>
@@ -967,10 +982,10 @@
       <c r="G12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="16" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1064,14 +1079,14 @@
         <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>37</v>
@@ -1081,7 +1096,7 @@
     <row r="17" spans="1:9" ht="33" customHeight="1" thickBot="1">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>23</v>
@@ -1093,11 +1108,11 @@
         <v>30</v>
       </c>
       <c r="F17" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>38</v>
@@ -1169,7 +1184,7 @@
     </row>
     <row r="21" spans="1:9" ht="16.8" customHeight="1" thickBot="1">
       <c r="A21" s="3"/>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1192,26 +1207,26 @@
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="15">
+      <c r="B22" s="18">
         <f>H5</f>
         <v>135</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="19">
         <f>SUM(E13:E19)</f>
-        <v>113</v>
-      </c>
-      <c r="D22" s="2">
+        <v>118</v>
+      </c>
+      <c r="D22" s="19">
         <f>SUM(F13:F19)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
+        <v>16</v>
+      </c>
+      <c r="E22" s="19">
         <f>C22-D22</f>
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="17">
+      <c r="G22" s="20">
         <f>B22-C22</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1298,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" ref="G26:G30" si="3">E26-F26</f>
+        <f t="shared" ref="G26:G29" si="3">E26-F26</f>
         <v>20</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -1423,7 +1438,7 @@
     </row>
     <row r="32" spans="1:9" ht="28.8" thickBot="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -1446,24 +1461,24 @@
       <c r="A33" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="18">
         <f>H6</f>
         <v>105</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="19">
         <f>SUM(E25:E30)</f>
         <v>63</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="19">
         <f>SUM(F25:F30)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="19">
         <f>C33-D33</f>
         <v>63</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="17">
+      <c r="F33" s="10"/>
+      <c r="G33" s="20">
         <f>B33-C33</f>
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
updated the planning, UML and documentation
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\ASP.NETCinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D759FD6-C199-4C34-85F0-9B35C8BDD5D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33454B1-E732-43F8-A118-2731AD28CF24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22E80722-1DB3-4D4A-B95F-931B24953C16}"/>
   </bookViews>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B06F840-217A-487E-A4A4-1D61301F5C6F}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -852,21 +852,21 @@
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5">
-        <v>43595</v>
+        <v>43596</v>
       </c>
       <c r="E6" s="5">
         <v>43616</v>
       </c>
       <c r="F6" s="14">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="G6" s="2">
         <v>35</v>
       </c>
       <c r="H6" s="14">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="13"/>
@@ -911,7 +911,7 @@
       </c>
       <c r="F8" s="14">
         <f>SUM(F2:F7)</f>
-        <v>19.142857142857142</v>
+        <v>19</v>
       </c>
       <c r="G8" s="2">
         <f>SUM(G2:G7)</f>
@@ -919,7 +919,7 @@
       </c>
       <c r="H8" s="14">
         <f>SUM(H2:H6)</f>
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="13"/>
@@ -1027,14 +1027,14 @@
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" ref="G14:G19" si="2">E14-F14</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>34</v>
@@ -1050,17 +1050,17 @@
         <v>24</v>
       </c>
       <c r="D15" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" s="2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>36</v>
@@ -1076,17 +1076,17 @@
         <v>22</v>
       </c>
       <c r="D16" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>37</v>
@@ -1105,14 +1105,14 @@
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F17" s="2">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>38</v>
@@ -1128,7 +1128,7 @@
         <v>25</v>
       </c>
       <c r="D18" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="2">
         <v>15</v>
@@ -1154,17 +1154,17 @@
         <v>17</v>
       </c>
       <c r="D19" s="8">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
         <v>4</v>
-      </c>
-      <c r="E19" s="2">
-        <v>8</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>40</v>
@@ -1213,20 +1213,20 @@
       </c>
       <c r="C22" s="19">
         <f>SUM(E13:E19)</f>
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D22" s="19">
         <f>SUM(F13:F19)</f>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E22" s="19">
         <f>C22-D22</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="20">
         <f>B22-C22</f>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1278,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="D25" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="2">
         <v>5</v>
@@ -1307,14 +1307,14 @@
         <v>1</v>
       </c>
       <c r="E26" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
       </c>
       <c r="G26" s="8">
         <f t="shared" ref="G26:G29" si="3">E26-F26</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>34</v>
@@ -1359,14 +1359,14 @@
         <v>3</v>
       </c>
       <c r="E28" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F28" s="3">
         <v>0</v>
       </c>
       <c r="G28" s="8">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>41</v>
@@ -1408,17 +1408,17 @@
         <v>32</v>
       </c>
       <c r="D30" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E30" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
       </c>
       <c r="G30" s="8">
         <f>E30-F30</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>43</v>
@@ -1463,11 +1463,11 @@
       </c>
       <c r="B33" s="18">
         <f>H6</f>
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C33" s="19">
         <f>SUM(E25:E30)</f>
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="D33" s="19">
         <f>SUM(F25:F30)</f>
@@ -1475,12 +1475,12 @@
       </c>
       <c r="E33" s="19">
         <f>C33-D33</f>
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="20">
         <f>B33-C33</f>
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>

</xml_diff>

<commit_message>
removed some spelling and grammar errors with the auto checker
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\ASP.NETCinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33454B1-E732-43F8-A118-2731AD28CF24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5724BB86-603B-41AD-9C1C-99C99BF164DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22E80722-1DB3-4D4A-B95F-931B24953C16}"/>
   </bookViews>
@@ -141,12 +141,6 @@
     <t>Waarom duurde het zo lang?</t>
   </si>
   <si>
-    <t>Dit is een redelijk breed onderwerp en ik heb nog niet precies bepaald aan welke onderdelen ik tijd wil gaan besteden. Daarom heb ik 20 uur hiervoor vrijgemaakt.</t>
-  </si>
-  <si>
-    <t>Dit zal niet extreem lastig worden maar voor het geval het moeilijker blijkt te zijn heb ik toch 10 uur vrij gemaakt.</t>
-  </si>
-  <si>
     <t>Ik zal een heel groot deel van de container opdracht moeten aanpassen of opnieuw moeten maken als ik de feedback van de docenten wil verwerken. Daarom heb ik erg veel tijd vrijgemaakt hiervoor.</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>Dit zal in de tussentijd gemaakt worden als het blijkt dat ik bepaalde dingen in mijn applicatie heb aangepast en als dat nog niet in mijn document staat.</t>
   </si>
   <si>
-    <t>Dit kan erg lang doorblijven gaan dus ik zet er een maximum van 10 uur voor deze sprint op.</t>
-  </si>
-  <si>
     <t>Ik weet niet zeker hoe lang dit gaat duren dus ik zal er niet te veel maar ook niet te weinig tijd voor vrijmaken.</t>
   </si>
   <si>
@@ -169,6 +160,15 @@
   </si>
   <si>
     <t>Bezig (Niet af)</t>
+  </si>
+  <si>
+    <t>Dit kan erg lang doorblijven gaan dus ik zet er een maximum van 15 uur voor deze sprint op.</t>
+  </si>
+  <si>
+    <t>Dit is een redelijk breed onderwerp en ik heb nog niet precies bepaald aan welke onderdelen ik tijd wil gaan besteden. Daarom heb ik 10 uur hiervoor vrijgemaakt.</t>
+  </si>
+  <si>
+    <t>Dit zal niet extreem lastig worden maar voor het geval het moeilijker blijkt te zijn heb ik toch 5 uur vrij gemaakt.</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B06F840-217A-487E-A4A4-1D61301F5C6F}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -899,7 +899,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1030,11 +1030,11 @@
         <v>30</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" ref="G14:G19" si="2">E14-F14</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>34</v>
@@ -1053,17 +1053,17 @@
         <v>4</v>
       </c>
       <c r="E15" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I15" s="3"/>
     </row>
@@ -1079,24 +1079,24 @@
         <v>4</v>
       </c>
       <c r="E16" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
       </c>
       <c r="G16" s="8">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="33" customHeight="1" thickBot="1">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>23</v>
@@ -1105,17 +1105,17 @@
         <v>1</v>
       </c>
       <c r="E17" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2">
         <v>23</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I17" s="3"/>
     </row>
@@ -1141,7 +1141,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I18" s="3"/>
     </row>
@@ -1154,20 +1154,20 @@
         <v>17</v>
       </c>
       <c r="D19" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I19" s="3"/>
     </row>
@@ -1213,20 +1213,20 @@
       </c>
       <c r="C22" s="19">
         <f>SUM(E13:E19)</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D22" s="19">
         <f>SUM(F13:F19)</f>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E22" s="19">
         <f>C22-D22</f>
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="20">
         <f>B22-C22</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -1307,14 +1307,14 @@
         <v>1</v>
       </c>
       <c r="E26" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
       </c>
       <c r="G26" s="8">
         <f t="shared" ref="G26:G29" si="3">E26-F26</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>34</v>
@@ -1333,17 +1333,17 @@
         <v>2</v>
       </c>
       <c r="E27" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
       </c>
       <c r="G27" s="8">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I27" s="3"/>
     </row>
@@ -1369,7 +1369,7 @@
         <v>15</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I28" s="3"/>
     </row>
@@ -1395,7 +1395,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I29" s="3"/>
     </row>
@@ -1421,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="C33" s="19">
         <f>SUM(E25:E30)</f>
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="D33" s="19">
         <f>SUM(F25:F30)</f>
@@ -1475,12 +1475,12 @@
       </c>
       <c r="E33" s="19">
         <f>C33-D33</f>
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="20">
         <f>B33-C33</f>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>

</xml_diff>

<commit_message>
query location moved, planning updated
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\source\repos\ZeusKingOfTheGods\ASP.NETCinema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\source\repos\ASP.NETCinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5724BB86-603B-41AD-9C1C-99C99BF164DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711D8FDE-B7E2-48EB-AB3D-D5C28015862A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22E80722-1DB3-4D4A-B95F-931B24953C16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{22E80722-1DB3-4D4A-B95F-931B24953C16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>Sprint</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Dit zal niet extreem lastig worden maar voor het geval het moeilijker blijkt te zijn heb ik toch 5 uur vrij gemaakt.</t>
+  </si>
+  <si>
+    <t>Container opdracht verbeteren</t>
   </si>
 </sst>
 </file>
@@ -176,9 +179,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -319,7 +322,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -362,7 +365,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,17 +377,17 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -400,7 +403,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -696,26 +699,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B06F840-217A-487E-A4A4-1D61301F5C6F}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="64.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="85" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" customWidth="1"/>
+    <col min="9" max="9" width="68.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="28.9" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +744,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:10" ht="16.2" customHeight="1" thickBot="1">
+    <row r="2" spans="1:10" ht="16.149999999999999" customHeight="1" thickBot="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -767,7 +770,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" ht="19.2" customHeight="1" thickBot="1">
+    <row r="3" spans="1:10" ht="19.149999999999999" customHeight="1" thickBot="1">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -793,7 +796,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="13"/>
     </row>
-    <row r="4" spans="1:10" ht="16.8" customHeight="1" thickBot="1">
+    <row r="4" spans="1:10" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -897,7 +900,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -924,7 +927,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -936,7 +939,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -948,7 +951,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -989,7 +992,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" customHeight="1" thickBot="1">
+    <row r="13" spans="1:10" ht="28.9" customHeight="1" thickBot="1">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
@@ -1015,7 +1018,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="28.2" customHeight="1" thickBot="1">
+    <row r="14" spans="1:10" ht="28.15" customHeight="1" thickBot="1">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>19</v>
@@ -1030,11 +1033,11 @@
         <v>30</v>
       </c>
       <c r="F14" s="2">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G14" s="8">
         <f t="shared" ref="G14:G19" si="2">E14-F14</f>
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>34</v>
@@ -1067,7 +1070,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="31.2" customHeight="1" thickBot="1">
+    <row r="16" spans="1:10" ht="31.15" customHeight="1" thickBot="1">
       <c r="A16" s="4"/>
       <c r="B16" s="4" t="s">
         <v>19</v>
@@ -1108,18 +1111,18 @@
         <v>50</v>
       </c>
       <c r="F17" s="2">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="29.4" customHeight="1" thickBot="1">
+    <row r="18" spans="1:9" ht="29.45" customHeight="1" thickBot="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>19</v>
@@ -1134,18 +1137,18 @@
         <v>15</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>37</v>
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="32.4" customHeight="1" thickBot="1">
+    <row r="19" spans="1:9" ht="32.450000000000003" customHeight="1" thickBot="1">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
         <v>19</v>
@@ -1160,18 +1163,18 @@
         <v>5</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1182,7 +1185,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="16.8" customHeight="1" thickBot="1">
+    <row r="21" spans="1:9" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A21" s="3"/>
       <c r="B21" s="15" t="s">
         <v>27</v>
@@ -1203,7 +1206,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="16.8" customHeight="1" thickBot="1">
+    <row r="22" spans="1:9" ht="16.899999999999999" customHeight="1" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>11</v>
       </c>
@@ -1217,11 +1220,11 @@
       </c>
       <c r="D22" s="19">
         <f>SUM(F13:F19)</f>
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="E22" s="19">
         <f>C22-D22</f>
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="20">
@@ -1231,7 +1234,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1269,7 +1272,7 @@
       </c>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="31.8" customHeight="1" thickBot="1">
+    <row r="25" spans="1:9" ht="31.9" customHeight="1" thickBot="1">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>19</v>
@@ -1295,7 +1298,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" ht="31.8" customHeight="1" thickBot="1">
+    <row r="26" spans="1:9" ht="31.9" customHeight="1" thickBot="1">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>19</v>
@@ -1313,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" ref="G26:G29" si="3">E26-F26</f>
+        <f t="shared" ref="G26:G30" si="3">E26-F26</f>
         <v>40</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -1321,7 +1324,7 @@
       </c>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" ht="29.4" customHeight="1" thickBot="1">
+    <row r="27" spans="1:9" ht="29.45" customHeight="1" thickBot="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>19</v>
@@ -1347,44 +1350,42 @@
       </c>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" ht="21" customHeight="1" thickBot="1">
+    <row r="28" spans="1:9" ht="29.45" customHeight="1" thickBot="1">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>30</v>
+      <c r="C28" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="D28" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F28" s="3">
         <v>0</v>
       </c>
       <c r="G28" s="8">
-        <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>43</v>
-      </c>
+        <f>E28-F28</f>
+        <v>25</v>
+      </c>
+      <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" ht="30.6" customHeight="1" thickBot="1">
+    <row r="29" spans="1:9" ht="21" customHeight="1" thickBot="1">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="8">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2">
         <v>15</v>
       </c>
       <c r="F29" s="3">
@@ -1395,109 +1396,135 @@
         <v>15</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" ht="28.8" thickBot="1">
+    <row r="30" spans="1:9" ht="30.6" customHeight="1" thickBot="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="8">
         <v>1</v>
       </c>
       <c r="E30" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F30" s="3">
         <v>0</v>
       </c>
       <c r="G30" s="8">
-        <f>E30-F30</f>
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" thickBot="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
         <v>10</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="8">
+        <f>E31-F31</f>
+        <v>10</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="28.8" thickBot="1">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:9" ht="30" thickBot="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A34" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="18">
+      <c r="B34" s="18">
         <f>H6</f>
         <v>100</v>
       </c>
-      <c r="C33" s="19">
-        <f>SUM(E25:E30)</f>
-        <v>95</v>
-      </c>
-      <c r="D33" s="19">
-        <f>SUM(F25:F30)</f>
+      <c r="C34" s="19">
+        <f>SUM(E25:E31)</f>
+        <v>120</v>
+      </c>
+      <c r="D34" s="19">
+        <f>SUM(F25:F31)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="19">
-        <f>C33-D33</f>
-        <v>95</v>
-      </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="20">
-        <f>B33-C33</f>
-        <v>5</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
+      <c r="E34" s="19">
+        <f>C34-D34</f>
+        <v>120</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="20">
+        <f>B34-C34</f>
+        <v>-20</v>
+      </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G25:G30">
+  <conditionalFormatting sqref="G25:G31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1509,7 +1536,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D30">
+  <conditionalFormatting sqref="D25:D31">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>